<commit_message>
update structure to an api approach
</commit_message>
<xml_diff>
--- a/data-raw/epu.xlsx
+++ b/data-raw/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="30">
   <si>
     <t>year</t>
   </si>
@@ -87,6 +87,15 @@
     <t>2020</t>
   </si>
   <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
     <t>Source: 'Measuring Economic Policy Uncertainty' by Scott Baker, Nicholas Bloom and Steven J. Davis at www.PolicyUncertainty.com.  These data can be used freely with attribution to the authors, the paper, and the website.</t>
   </si>
   <si>
@@ -137,7 +146,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C276"/>
+  <dimension ref="A1:C305"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -145,10 +154,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
@@ -159,7 +168,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="0">
-        <v>114.2330322265625</v>
+        <v>114.23303041919498</v>
       </c>
     </row>
     <row r="3">
@@ -170,7 +179,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0">
-        <v>71.152473449707031</v>
+        <v>71.152468112217733</v>
       </c>
     </row>
     <row r="4">
@@ -181,7 +190,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="0">
-        <v>148.08653259277344</v>
+        <v>148.08653465656573</v>
       </c>
     </row>
     <row r="5">
@@ -192,7 +201,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="0">
-        <v>146.97679138183594</v>
+        <v>146.97678918911495</v>
       </c>
     </row>
     <row r="6">
@@ -203,7 +212,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="0">
-        <v>111.51500701904297</v>
+        <v>111.51501101796822</v>
       </c>
     </row>
     <row r="7">
@@ -214,7 +223,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="0">
-        <v>85.492919921875</v>
+        <v>85.492917317480106</v>
       </c>
     </row>
     <row r="8">
@@ -225,7 +234,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="0">
-        <v>180.79301452636719</v>
+        <v>180.79302078297567</v>
       </c>
     </row>
     <row r="9">
@@ -236,7 +245,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="0">
-        <v>140.59883117675781</v>
+        <v>140.59883854349383</v>
       </c>
     </row>
     <row r="10">
@@ -247,7 +256,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="0">
-        <v>193.86285400390625</v>
+        <v>193.86284404128827</v>
       </c>
     </row>
     <row r="11">
@@ -258,7 +267,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="0">
-        <v>256.06808471679687</v>
+        <v>256.06809124079552</v>
       </c>
     </row>
     <row r="12">
@@ -269,7 +278,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="0">
-        <v>172.85871887207031</v>
+        <v>172.85871532726372</v>
       </c>
     </row>
     <row r="13">
@@ -280,7 +289,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="0">
-        <v>123.54463195800781</v>
+        <v>123.54462447386712</v>
       </c>
     </row>
     <row r="14">
@@ -291,7 +300,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="0">
-        <v>99.624839782714844</v>
+        <v>99.624838290417301</v>
       </c>
     </row>
     <row r="15">
@@ -302,7 +311,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="0">
-        <v>89.3013916015625</v>
+        <v>89.301390805313901</v>
       </c>
     </row>
     <row r="16">
@@ -313,7 +322,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="0">
-        <v>84.704429626464844</v>
+        <v>84.704431375507454</v>
       </c>
     </row>
     <row r="17">
@@ -324,7 +333,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="0">
-        <v>63.930248260498047</v>
+        <v>63.930248201578557</v>
       </c>
     </row>
     <row r="18">
@@ -335,7 +344,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="0">
-        <v>71.887985229492187</v>
+        <v>71.887983294516644</v>
       </c>
     </row>
     <row r="19">
@@ -346,7 +355,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="0">
-        <v>52.256729125976563</v>
+        <v>52.256729242724006</v>
       </c>
     </row>
     <row r="20">
@@ -357,7 +366,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="0">
-        <v>81.232292175292969</v>
+        <v>81.232297333847839</v>
       </c>
     </row>
     <row r="21">
@@ -368,7 +377,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="0">
-        <v>72.576705932617188</v>
+        <v>72.576704428693134</v>
       </c>
     </row>
     <row r="22">
@@ -379,7 +388,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="0">
-        <v>67.1275634765625</v>
+        <v>67.127564501344565</v>
       </c>
     </row>
     <row r="23">
@@ -390,7 +399,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="0">
-        <v>123.12413024902344</v>
+        <v>123.12413166974538</v>
       </c>
     </row>
     <row r="24">
@@ -401,7 +410,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="0">
-        <v>26.846799850463867</v>
+        <v>26.84680026099262</v>
       </c>
     </row>
     <row r="25">
@@ -412,7 +421,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="0">
-        <v>48.689983367919922</v>
+        <v>48.689985458213094</v>
       </c>
     </row>
     <row r="26">
@@ -423,7 +432,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="0">
-        <v>53.748451232910156</v>
+        <v>53.748451022419943</v>
       </c>
     </row>
     <row r="27">
@@ -434,7 +443,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="0">
-        <v>58.396511077880859</v>
+        <v>58.396510954430312</v>
       </c>
     </row>
     <row r="28">
@@ -445,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="0">
-        <v>61.960391998291016</v>
+        <v>61.960392681100373</v>
       </c>
     </row>
     <row r="29">
@@ -456,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="0">
-        <v>114.01042938232422</v>
+        <v>114.01042927352911</v>
       </c>
     </row>
     <row r="30">
@@ -467,7 +476,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="0">
-        <v>46.368324279785156</v>
+        <v>46.368325435466247</v>
       </c>
     </row>
     <row r="31">
@@ -478,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="0">
-        <v>133.21640014648437</v>
+        <v>133.21640062369883</v>
       </c>
     </row>
     <row r="32">
@@ -489,7 +498,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="0">
-        <v>73.706695556640625</v>
+        <v>73.706699857582223</v>
       </c>
     </row>
     <row r="33">
@@ -500,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="0">
-        <v>42.748378753662109</v>
+        <v>42.748375788974677</v>
       </c>
     </row>
     <row r="34">
@@ -511,7 +520,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="0">
-        <v>55.577869415283203</v>
+        <v>55.577872298404039</v>
       </c>
     </row>
     <row r="35">
@@ -522,7 +531,7 @@
         <v>10</v>
       </c>
       <c r="C35" s="0">
-        <v>55.821765899658203</v>
+        <v>55.821764612416644</v>
       </c>
     </row>
     <row r="36">
@@ -533,7 +542,7 @@
         <v>11</v>
       </c>
       <c r="C36" s="0">
-        <v>68.99102783203125</v>
+        <v>68.991031741151005</v>
       </c>
     </row>
     <row r="37">
@@ -544,7 +553,7 @@
         <v>12</v>
       </c>
       <c r="C37" s="0">
-        <v>66.450172424316406</v>
+        <v>66.450174706116044</v>
       </c>
     </row>
     <row r="38">
@@ -555,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="0">
-        <v>38.407833099365234</v>
+        <v>38.407833958642684</v>
       </c>
     </row>
     <row r="39">
@@ -566,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="0">
-        <v>56.693271636962891</v>
+        <v>56.693271350649312</v>
       </c>
     </row>
     <row r="40">
@@ -577,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="0">
-        <v>91.642860412597656</v>
+        <v>91.642864752455026</v>
       </c>
     </row>
     <row r="41">
@@ -588,7 +597,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="0">
-        <v>100.98927307128906</v>
+        <v>100.98927389864957</v>
       </c>
     </row>
     <row r="42">
@@ -599,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="0">
-        <v>98.2562255859375</v>
+        <v>98.256230864099578</v>
       </c>
     </row>
     <row r="43">
@@ -610,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="C43" s="0">
-        <v>74.842735290527344</v>
+        <v>74.842735742282386</v>
       </c>
     </row>
     <row r="44">
@@ -621,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="C44" s="0">
-        <v>66.38372802734375</v>
+        <v>66.38372519061484</v>
       </c>
     </row>
     <row r="45">
@@ -632,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="C45" s="0">
-        <v>105.13270568847656</v>
+        <v>105.13269947080015</v>
       </c>
     </row>
     <row r="46">
@@ -643,7 +652,7 @@
         <v>9</v>
       </c>
       <c r="C46" s="0">
-        <v>205.25697326660156</v>
+        <v>205.25697487631768</v>
       </c>
     </row>
     <row r="47">
@@ -654,7 +663,7 @@
         <v>10</v>
       </c>
       <c r="C47" s="0">
-        <v>158.72160339355469</v>
+        <v>158.72159980318426</v>
       </c>
     </row>
     <row r="48">
@@ -665,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="C48" s="0">
-        <v>146.11531066894531</v>
+        <v>146.11531254475</v>
       </c>
     </row>
     <row r="49">
@@ -676,7 +685,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="0">
-        <v>108.11412811279297</v>
+        <v>108.11412471348061</v>
       </c>
     </row>
     <row r="50">
@@ -687,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="0">
-        <v>85.506576538085938</v>
+        <v>85.506579174754521</v>
       </c>
     </row>
     <row r="51">
@@ -698,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="0">
-        <v>70.793487548828125</v>
+        <v>70.793482785977702</v>
       </c>
     </row>
     <row r="52">
@@ -709,7 +718,7 @@
         <v>3</v>
       </c>
       <c r="C52" s="0">
-        <v>76.328315734863281</v>
+        <v>76.328319642242249</v>
       </c>
     </row>
     <row r="53">
@@ -720,7 +729,7 @@
         <v>4</v>
       </c>
       <c r="C53" s="0">
-        <v>78.088180541992188</v>
+        <v>78.088182950900872</v>
       </c>
     </row>
     <row r="54">
@@ -731,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="0">
-        <v>67.406356811523438</v>
+        <v>67.406353692455028</v>
       </c>
     </row>
     <row r="55">
@@ -742,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="C55" s="0">
-        <v>86.87921142578125</v>
+        <v>86.879203610639379</v>
       </c>
     </row>
     <row r="56">
@@ -753,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="0">
-        <v>88.472572326660156</v>
+        <v>88.472571429943144</v>
       </c>
     </row>
     <row r="57">
@@ -764,7 +773,7 @@
         <v>8</v>
       </c>
       <c r="C57" s="0">
-        <v>93.7239990234375</v>
+        <v>93.723994884644043</v>
       </c>
     </row>
     <row r="58">
@@ -775,7 +784,7 @@
         <v>9</v>
       </c>
       <c r="C58" s="0">
-        <v>127.27272796630859</v>
+        <v>127.27273057482194</v>
       </c>
     </row>
     <row r="59">
@@ -786,7 +795,7 @@
         <v>10</v>
       </c>
       <c r="C59" s="0">
-        <v>108.42975616455078</v>
+        <v>108.4297542573948</v>
       </c>
     </row>
     <row r="60">
@@ -797,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="C60" s="0">
-        <v>115.09958648681641</v>
+        <v>115.09958348207847</v>
       </c>
     </row>
     <row r="61">
@@ -808,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="C61" s="0">
-        <v>118.64259338378906</v>
+        <v>118.64259248874143</v>
       </c>
     </row>
     <row r="62">
@@ -819,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="0">
-        <v>146.05941772460937</v>
+        <v>146.05941292203249</v>
       </c>
     </row>
     <row r="63">
@@ -830,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="0">
-        <v>178.73886108398437</v>
+        <v>178.73887349178023</v>
       </c>
     </row>
     <row r="64">
@@ -841,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="C64" s="0">
-        <v>174.97273254394531</v>
+        <v>174.97273471435085</v>
       </c>
     </row>
     <row r="65">
@@ -852,7 +861,7 @@
         <v>4</v>
       </c>
       <c r="C65" s="0">
-        <v>153.50643920898437</v>
+        <v>153.50644782837878</v>
       </c>
     </row>
     <row r="66">
@@ -863,7 +872,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="0">
-        <v>93.713760375976563</v>
+        <v>93.713759198405427</v>
       </c>
     </row>
     <row r="67">
@@ -874,7 +883,7 @@
         <v>6</v>
       </c>
       <c r="C67" s="0">
-        <v>125.0064697265625</v>
+        <v>125.00647484433625</v>
       </c>
     </row>
     <row r="68">
@@ -885,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="C68" s="0">
-        <v>80.936637878417969</v>
+        <v>80.936638413478462</v>
       </c>
     </row>
     <row r="69">
@@ -896,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="C69" s="0">
-        <v>83.362625122070313</v>
+        <v>83.362627004704052</v>
       </c>
     </row>
     <row r="70">
@@ -907,7 +916,7 @@
         <v>9</v>
       </c>
       <c r="C70" s="0">
-        <v>65.412857055664063</v>
+        <v>65.412854559766302</v>
       </c>
     </row>
     <row r="71">
@@ -918,7 +927,7 @@
         <v>10</v>
       </c>
       <c r="C71" s="0">
-        <v>62.298290252685547</v>
+        <v>62.298289449657176</v>
       </c>
     </row>
     <row r="72">
@@ -929,7 +938,7 @@
         <v>11</v>
       </c>
       <c r="C72" s="0">
-        <v>78.4478759765625</v>
+        <v>78.4478801122807</v>
       </c>
     </row>
     <row r="73">
@@ -940,7 +949,7 @@
         <v>12</v>
       </c>
       <c r="C73" s="0">
-        <v>46.291194915771484</v>
+        <v>46.291193655705612</v>
       </c>
     </row>
     <row r="74">
@@ -951,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="0">
-        <v>24.035942077636719</v>
+        <v>24.0359419445406</v>
       </c>
     </row>
     <row r="75">
@@ -962,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="0">
-        <v>57.130153656005859</v>
+        <v>57.130154355236499</v>
       </c>
     </row>
     <row r="76">
@@ -973,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="0">
-        <v>61.884700775146484</v>
+        <v>61.884703940211296</v>
       </c>
     </row>
     <row r="77">
@@ -984,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="C77" s="0">
-        <v>38.552352905273438</v>
+        <v>38.552354422083354</v>
       </c>
     </row>
     <row r="78">
@@ -995,7 +1004,7 @@
         <v>5</v>
       </c>
       <c r="C78" s="0">
-        <v>42.882164001464844</v>
+        <v>42.88216533306619</v>
       </c>
     </row>
     <row r="79">
@@ -1006,7 +1015,7 @@
         <v>6</v>
       </c>
       <c r="C79" s="0">
-        <v>49.439136505126953</v>
+        <v>49.439137156664231</v>
       </c>
     </row>
     <row r="80">
@@ -1017,7 +1026,7 @@
         <v>7</v>
       </c>
       <c r="C80" s="0">
-        <v>52.617275238037109</v>
+        <v>52.617274390594723</v>
       </c>
     </row>
     <row r="81">
@@ -1028,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="C81" s="0">
-        <v>39.393718719482422</v>
+        <v>39.393721041190858</v>
       </c>
     </row>
     <row r="82">
@@ -1039,7 +1048,7 @@
         <v>9</v>
       </c>
       <c r="C82" s="0">
-        <v>49.166225433349609</v>
+        <v>49.166223902677764</v>
       </c>
     </row>
     <row r="83">
@@ -1050,7 +1059,7 @@
         <v>10</v>
       </c>
       <c r="C83" s="0">
-        <v>67.129158020019531</v>
+        <v>67.129160866436038</v>
       </c>
     </row>
     <row r="84">
@@ -1061,7 +1070,7 @@
         <v>11</v>
       </c>
       <c r="C84" s="0">
-        <v>68.726028442382813</v>
+        <v>68.726025959774617</v>
       </c>
     </row>
     <row r="85">
@@ -1072,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="C85" s="0">
-        <v>44.909515380859375</v>
+        <v>44.909516282941226</v>
       </c>
     </row>
     <row r="86">
@@ -1083,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="0">
-        <v>43.989646911621094</v>
+        <v>43.989646993249359</v>
       </c>
     </row>
     <row r="87">
@@ -1094,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="0">
-        <v>39.645351409912109</v>
+        <v>39.64534947881436</v>
       </c>
     </row>
     <row r="88">
@@ -1105,7 +1114,7 @@
         <v>3</v>
       </c>
       <c r="C88" s="0">
-        <v>34.078708648681641</v>
+        <v>34.07870982308976</v>
       </c>
     </row>
     <row r="89">
@@ -1116,7 +1125,7 @@
         <v>4</v>
       </c>
       <c r="C89" s="0">
-        <v>69.05712890625</v>
+        <v>69.057126421663469</v>
       </c>
     </row>
     <row r="90">
@@ -1127,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="C90" s="0">
-        <v>71.771087646484375</v>
+        <v>71.771089573397958</v>
       </c>
     </row>
     <row r="91">
@@ -1138,7 +1147,7 @@
         <v>6</v>
       </c>
       <c r="C91" s="0">
-        <v>59.403873443603516</v>
+        <v>59.403874719354278</v>
       </c>
     </row>
     <row r="92">
@@ -1149,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="C92" s="0">
-        <v>47.414012908935547</v>
+        <v>47.414013411934278</v>
       </c>
     </row>
     <row r="93">
@@ -1160,7 +1169,7 @@
         <v>8</v>
       </c>
       <c r="C93" s="0">
-        <v>48.541706085205078</v>
+        <v>48.54170562625211</v>
       </c>
     </row>
     <row r="94">
@@ -1171,7 +1180,7 @@
         <v>9</v>
       </c>
       <c r="C94" s="0">
-        <v>70.332473754882813</v>
+        <v>70.332476662916861</v>
       </c>
     </row>
     <row r="95">
@@ -1182,7 +1191,7 @@
         <v>10</v>
       </c>
       <c r="C95" s="0">
-        <v>40.613033294677734</v>
+        <v>40.613034313794714</v>
       </c>
     </row>
     <row r="96">
@@ -1193,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="C96" s="0">
-        <v>47.559238433837891</v>
+        <v>47.559237062280005</v>
       </c>
     </row>
     <row r="97">
@@ -1204,7 +1213,7 @@
         <v>12</v>
       </c>
       <c r="C97" s="0">
-        <v>33.106582641601563</v>
+        <v>33.10658195369718</v>
       </c>
     </row>
     <row r="98">
@@ -1215,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="0">
-        <v>44.040050506591797</v>
+        <v>44.040050065155981</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="C99" s="0">
-        <v>37.132061004638672</v>
+        <v>37.132061545598454</v>
       </c>
     </row>
     <row r="100">
@@ -1237,7 +1246,7 @@
         <v>3</v>
       </c>
       <c r="C100" s="0">
-        <v>42.456447601318359</v>
+        <v>42.456446706105879</v>
       </c>
     </row>
     <row r="101">
@@ -1248,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="C101" s="0">
-        <v>37.08660888671875</v>
+        <v>37.086608110653827</v>
       </c>
     </row>
     <row r="102">
@@ -1259,7 +1268,7 @@
         <v>5</v>
       </c>
       <c r="C102" s="0">
-        <v>74.022674560546875</v>
+        <v>74.022673592114302</v>
       </c>
     </row>
     <row r="103">
@@ -1270,7 +1279,7 @@
         <v>6</v>
       </c>
       <c r="C103" s="0">
-        <v>59.820568084716797</v>
+        <v>59.820568976535263</v>
       </c>
     </row>
     <row r="104">
@@ -1281,7 +1290,7 @@
         <v>7</v>
       </c>
       <c r="C104" s="0">
-        <v>47.543785095214844</v>
+        <v>47.543782394855668</v>
       </c>
     </row>
     <row r="105">
@@ -1292,7 +1301,7 @@
         <v>8</v>
       </c>
       <c r="C105" s="0">
-        <v>67.213226318359375</v>
+        <v>67.213228709248042</v>
       </c>
     </row>
     <row r="106">
@@ -1303,7 +1312,7 @@
         <v>9</v>
       </c>
       <c r="C106" s="0">
-        <v>56.234481811523438</v>
+        <v>56.234482774648797</v>
       </c>
     </row>
     <row r="107">
@@ -1314,7 +1323,7 @@
         <v>10</v>
       </c>
       <c r="C107" s="0">
-        <v>65.255081176757812</v>
+        <v>65.255080007947058</v>
       </c>
     </row>
     <row r="108">
@@ -1325,7 +1334,7 @@
         <v>11</v>
       </c>
       <c r="C108" s="0">
-        <v>59.490592956542969</v>
+        <v>59.49058917096486</v>
       </c>
     </row>
     <row r="109">
@@ -1336,7 +1345,7 @@
         <v>12</v>
       </c>
       <c r="C109" s="0">
-        <v>64.488700866699219</v>
+        <v>64.488699636232127</v>
       </c>
     </row>
     <row r="110">
@@ -1347,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="C110" s="0">
-        <v>49.232185363769531</v>
+        <v>49.232184122049397</v>
       </c>
     </row>
     <row r="111">
@@ -1358,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="C111" s="0">
-        <v>53.071933746337891</v>
+        <v>53.071933804627889</v>
       </c>
     </row>
     <row r="112">
@@ -1369,7 +1378,7 @@
         <v>3</v>
       </c>
       <c r="C112" s="0">
-        <v>77.055221557617188</v>
+        <v>77.055227733903877</v>
       </c>
     </row>
     <row r="113">
@@ -1380,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="C113" s="0">
-        <v>60.96484375</v>
+        <v>60.964843473864342</v>
       </c>
     </row>
     <row r="114">
@@ -1391,7 +1400,7 @@
         <v>5</v>
       </c>
       <c r="C114" s="0">
-        <v>66.573944091796875</v>
+        <v>66.573947273860682</v>
       </c>
     </row>
     <row r="115">
@@ -1402,7 +1411,7 @@
         <v>6</v>
       </c>
       <c r="C115" s="0">
-        <v>53.468608856201172</v>
+        <v>53.468607020779125</v>
       </c>
     </row>
     <row r="116">
@@ -1413,7 +1422,7 @@
         <v>7</v>
       </c>
       <c r="C116" s="0">
-        <v>48.757678985595703</v>
+        <v>48.757679221451504</v>
       </c>
     </row>
     <row r="117">
@@ -1424,7 +1433,7 @@
         <v>8</v>
       </c>
       <c r="C117" s="0">
-        <v>77.388679504394531</v>
+        <v>77.388682544021719</v>
       </c>
     </row>
     <row r="118">
@@ -1435,7 +1444,7 @@
         <v>9</v>
       </c>
       <c r="C118" s="0">
-        <v>132.26576232910156</v>
+        <v>132.26575539424326</v>
       </c>
     </row>
     <row r="119">
@@ -1446,7 +1455,7 @@
         <v>10</v>
       </c>
       <c r="C119" s="0">
-        <v>91.692916870117188</v>
+        <v>91.692920345072537</v>
       </c>
     </row>
     <row r="120">
@@ -1457,7 +1466,7 @@
         <v>11</v>
       </c>
       <c r="C120" s="0">
-        <v>131.62321472167969</v>
+        <v>131.62321770144564</v>
       </c>
     </row>
     <row r="121">
@@ -1468,7 +1477,7 @@
         <v>12</v>
       </c>
       <c r="C121" s="0">
-        <v>150.87321472167969</v>
+        <v>150.8732135162181</v>
       </c>
     </row>
     <row r="122">
@@ -1479,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="0">
-        <v>138.57289123535156</v>
+        <v>138.57289473235426</v>
       </c>
     </row>
     <row r="123">
@@ -1490,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="C123" s="0">
-        <v>145.78488159179687</v>
+        <v>145.78488588875288</v>
       </c>
     </row>
     <row r="124">
@@ -1501,7 +1510,7 @@
         <v>3</v>
       </c>
       <c r="C124" s="0">
-        <v>168.74942016601562</v>
+        <v>168.74941890266629</v>
       </c>
     </row>
     <row r="125">
@@ -1512,7 +1521,7 @@
         <v>4</v>
       </c>
       <c r="C125" s="0">
-        <v>129.51087951660156</v>
+        <v>129.51088529834928</v>
       </c>
     </row>
     <row r="126">
@@ -1523,7 +1532,7 @@
         <v>5</v>
       </c>
       <c r="C126" s="0">
-        <v>112.51808166503906</v>
+        <v>112.51807597636849</v>
       </c>
     </row>
     <row r="127">
@@ -1534,7 +1543,7 @@
         <v>6</v>
       </c>
       <c r="C127" s="0">
-        <v>107.00999450683594</v>
+        <v>107.00998790223383</v>
       </c>
     </row>
     <row r="128">
@@ -1545,7 +1554,7 @@
         <v>7</v>
       </c>
       <c r="C128" s="0">
-        <v>113.38642883300781</v>
+        <v>113.38642811958277</v>
       </c>
     </row>
     <row r="129">
@@ -1556,7 +1565,7 @@
         <v>8</v>
       </c>
       <c r="C129" s="0">
-        <v>143.64463806152344</v>
+        <v>143.64464702090251</v>
       </c>
     </row>
     <row r="130">
@@ -1567,7 +1576,7 @@
         <v>9</v>
       </c>
       <c r="C130" s="0">
-        <v>191.05964660644531</v>
+        <v>191.05963498096241</v>
       </c>
     </row>
     <row r="131">
@@ -1578,7 +1587,7 @@
         <v>10</v>
       </c>
       <c r="C131" s="0">
-        <v>242.234375</v>
+        <v>242.23438012932465</v>
       </c>
     </row>
     <row r="132">
@@ -1589,7 +1598,7 @@
         <v>11</v>
       </c>
       <c r="C132" s="0">
-        <v>169.54904174804687</v>
+        <v>169.54905468701816</v>
       </c>
     </row>
     <row r="133">
@@ -1600,7 +1609,7 @@
         <v>12</v>
       </c>
       <c r="C133" s="0">
-        <v>123.49229431152344</v>
+        <v>123.49229337979028</v>
       </c>
     </row>
     <row r="134">
@@ -1611,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="C134" s="0">
-        <v>129.44589233398438</v>
+        <v>129.44590205794026</v>
       </c>
     </row>
     <row r="135">
@@ -1622,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="C135" s="0">
-        <v>129.95285034179687</v>
+        <v>129.95284607940246</v>
       </c>
     </row>
     <row r="136">
@@ -1633,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="C136" s="0">
-        <v>111.89681243896484</v>
+        <v>111.89680762313428</v>
       </c>
     </row>
     <row r="137">
@@ -1644,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="0">
-        <v>111.6890869140625</v>
+        <v>111.68908181978891</v>
       </c>
     </row>
     <row r="138">
@@ -1655,7 +1664,7 @@
         <v>5</v>
       </c>
       <c r="C138" s="0">
-        <v>116.61088562011719</v>
+        <v>116.61089085999414</v>
       </c>
     </row>
     <row r="139">
@@ -1666,7 +1675,7 @@
         <v>6</v>
       </c>
       <c r="C139" s="0">
-        <v>154.18637084960937</v>
+        <v>154.18635733037533</v>
       </c>
     </row>
     <row r="140">
@@ -1677,7 +1686,7 @@
         <v>7</v>
       </c>
       <c r="C140" s="0">
-        <v>128.96145629882813</v>
+        <v>128.96145456031053</v>
       </c>
     </row>
     <row r="141">
@@ -1688,7 +1697,7 @@
         <v>8</v>
       </c>
       <c r="C141" s="0">
-        <v>117.74832153320312</v>
+        <v>117.74832179758042</v>
       </c>
     </row>
     <row r="142">
@@ -1699,7 +1708,7 @@
         <v>9</v>
       </c>
       <c r="C142" s="0">
-        <v>100.07635498046875</v>
+        <v>100.0763504077331</v>
       </c>
     </row>
     <row r="143">
@@ -1710,7 +1719,7 @@
         <v>10</v>
       </c>
       <c r="C143" s="0">
-        <v>107.54240417480469</v>
+        <v>107.54240446531122</v>
       </c>
     </row>
     <row r="144">
@@ -1721,7 +1730,7 @@
         <v>11</v>
       </c>
       <c r="C144" s="0">
-        <v>107.57199859619141</v>
+        <v>107.57200130311233</v>
       </c>
     </row>
     <row r="145">
@@ -1732,7 +1741,7 @@
         <v>12</v>
       </c>
       <c r="C145" s="0">
-        <v>135.97782897949219</v>
+        <v>135.97782174570824</v>
       </c>
     </row>
     <row r="146">
@@ -1743,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="C146" s="0">
-        <v>148.26554870605469</v>
+        <v>148.26556162676309</v>
       </c>
     </row>
     <row r="147">
@@ -1754,7 +1763,7 @@
         <v>2</v>
       </c>
       <c r="C147" s="0">
-        <v>143.34239196777344</v>
+        <v>143.34239608678251</v>
       </c>
     </row>
     <row r="148">
@@ -1765,7 +1774,7 @@
         <v>3</v>
       </c>
       <c r="C148" s="0">
-        <v>160.08869934082031</v>
+        <v>160.08868904162972</v>
       </c>
     </row>
     <row r="149">
@@ -1776,7 +1785,7 @@
         <v>4</v>
       </c>
       <c r="C149" s="0">
-        <v>161.00445556640625</v>
+        <v>161.00445943010854</v>
       </c>
     </row>
     <row r="150">
@@ -1787,7 +1796,7 @@
         <v>5</v>
       </c>
       <c r="C150" s="0">
-        <v>243.53857421875</v>
+        <v>243.53857801491344</v>
       </c>
     </row>
     <row r="151">
@@ -1798,7 +1807,7 @@
         <v>6</v>
       </c>
       <c r="C151" s="0">
-        <v>184.01828002929687</v>
+        <v>184.0182788836257</v>
       </c>
     </row>
     <row r="152">
@@ -1809,7 +1818,7 @@
         <v>7</v>
       </c>
       <c r="C152" s="0">
-        <v>142.86163330078125</v>
+        <v>142.86163286041818</v>
       </c>
     </row>
     <row r="153">
@@ -1820,7 +1829,7 @@
         <v>8</v>
       </c>
       <c r="C153" s="0">
-        <v>165.98422241210937</v>
+        <v>165.98422462934116</v>
       </c>
     </row>
     <row r="154">
@@ -1831,7 +1840,7 @@
         <v>9</v>
       </c>
       <c r="C154" s="0">
-        <v>127.90261840820313</v>
+        <v>127.90262125152725</v>
       </c>
     </row>
     <row r="155">
@@ -1842,7 +1851,7 @@
         <v>10</v>
       </c>
       <c r="C155" s="0">
-        <v>177.80287170410156</v>
+        <v>177.80286471621724</v>
       </c>
     </row>
     <row r="156">
@@ -1853,7 +1862,7 @@
         <v>11</v>
       </c>
       <c r="C156" s="0">
-        <v>153.24842834472656</v>
+        <v>153.24843338306422</v>
       </c>
     </row>
     <row r="157">
@@ -1864,7 +1873,7 @@
         <v>12</v>
       </c>
       <c r="C157" s="0">
-        <v>122.77899169921875</v>
+        <v>122.77899240938301</v>
       </c>
     </row>
     <row r="158">
@@ -1875,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="C158" s="0">
-        <v>123.68014526367187</v>
+        <v>123.680147938887</v>
       </c>
     </row>
     <row r="159">
@@ -1886,7 +1895,7 @@
         <v>2</v>
       </c>
       <c r="C159" s="0">
-        <v>119.12128448486328</v>
+        <v>119.12127850168046</v>
       </c>
     </row>
     <row r="160">
@@ -1897,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="C160" s="0">
-        <v>131.42254638671875</v>
+        <v>131.42253843387149</v>
       </c>
     </row>
     <row r="161">
@@ -1908,7 +1917,7 @@
         <v>4</v>
       </c>
       <c r="C161" s="0">
-        <v>97.936988830566406</v>
+        <v>97.93698999814309</v>
       </c>
     </row>
     <row r="162">
@@ -1919,7 +1928,7 @@
         <v>5</v>
       </c>
       <c r="C162" s="0">
-        <v>94.244071960449219</v>
+        <v>94.244068778262516</v>
       </c>
     </row>
     <row r="163">
@@ -1930,7 +1939,7 @@
         <v>6</v>
       </c>
       <c r="C163" s="0">
-        <v>122.69766998291016</v>
+        <v>122.6976663955935</v>
       </c>
     </row>
     <row r="164">
@@ -1941,7 +1950,7 @@
         <v>7</v>
       </c>
       <c r="C164" s="0">
-        <v>149.02828979492187</v>
+        <v>149.02829406668391</v>
       </c>
     </row>
     <row r="165">
@@ -1952,7 +1961,7 @@
         <v>8</v>
       </c>
       <c r="C165" s="0">
-        <v>177.75312805175781</v>
+        <v>177.75312265089235</v>
       </c>
     </row>
     <row r="166">
@@ -1963,7 +1972,7 @@
         <v>9</v>
       </c>
       <c r="C166" s="0">
-        <v>153.32763671875</v>
+        <v>153.32764352624784</v>
       </c>
     </row>
     <row r="167">
@@ -1974,7 +1983,7 @@
         <v>10</v>
       </c>
       <c r="C167" s="0">
-        <v>149.69090270996094</v>
+        <v>149.69090675465347</v>
       </c>
     </row>
     <row r="168">
@@ -1985,7 +1994,7 @@
         <v>11</v>
       </c>
       <c r="C168" s="0">
-        <v>209.89849853515625</v>
+        <v>209.89849346585174</v>
       </c>
     </row>
     <row r="169">
@@ -1996,7 +2005,7 @@
         <v>12</v>
       </c>
       <c r="C169" s="0">
-        <v>140.62797546386719</v>
+        <v>140.62797929349495</v>
       </c>
     </row>
     <row r="170">
@@ -2007,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="C170" s="0">
-        <v>137.26155090332031</v>
+        <v>137.26155402113505</v>
       </c>
     </row>
     <row r="171">
@@ -2018,7 +2027,7 @@
         <v>2</v>
       </c>
       <c r="C171" s="0">
-        <v>132.02021789550781</v>
+        <v>132.0202282564008</v>
       </c>
     </row>
     <row r="172">
@@ -2029,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="C172" s="0">
-        <v>103.72963714599609</v>
+        <v>103.72963719791315</v>
       </c>
     </row>
     <row r="173">
@@ -2040,7 +2049,7 @@
         <v>4</v>
       </c>
       <c r="C173" s="0">
-        <v>109.31269073486328</v>
+        <v>109.31269219071331</v>
       </c>
     </row>
     <row r="174">
@@ -2051,7 +2060,7 @@
         <v>5</v>
       </c>
       <c r="C174" s="0">
-        <v>151.78517150878906</v>
+        <v>151.78517880787442</v>
       </c>
     </row>
     <row r="175">
@@ -2062,7 +2071,7 @@
         <v>6</v>
       </c>
       <c r="C175" s="0">
-        <v>169.64906311035156</v>
+        <v>169.64907552579561</v>
       </c>
     </row>
     <row r="176">
@@ -2073,7 +2082,7 @@
         <v>7</v>
       </c>
       <c r="C176" s="0">
-        <v>129.98323059082031</v>
+        <v>129.98323050053759</v>
       </c>
     </row>
     <row r="177">
@@ -2084,7 +2093,7 @@
         <v>8</v>
       </c>
       <c r="C177" s="0">
-        <v>98.178688049316406</v>
+        <v>98.178687632659731</v>
       </c>
     </row>
     <row r="178">
@@ -2095,7 +2104,7 @@
         <v>9</v>
       </c>
       <c r="C178" s="0">
-        <v>124.43543243408203</v>
+        <v>124.43543264760135</v>
       </c>
     </row>
     <row r="179">
@@ -2106,7 +2115,7 @@
         <v>10</v>
       </c>
       <c r="C179" s="0">
-        <v>153.99227905273437</v>
+        <v>153.99229062161274</v>
       </c>
     </row>
     <row r="180">
@@ -2117,7 +2126,7 @@
         <v>11</v>
       </c>
       <c r="C180" s="0">
-        <v>162.10096740722656</v>
+        <v>162.1009636904767</v>
       </c>
     </row>
     <row r="181">
@@ -2128,7 +2137,7 @@
         <v>12</v>
       </c>
       <c r="C181" s="0">
-        <v>140.64390563964844</v>
+        <v>140.64389927578668</v>
       </c>
     </row>
     <row r="182">
@@ -2139,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="C182" s="0">
-        <v>187.77023315429687</v>
+        <v>187.77022088412104</v>
       </c>
     </row>
     <row r="183">
@@ -2150,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="C183" s="0">
-        <v>97.381301879882813</v>
+        <v>97.381306471276645</v>
       </c>
     </row>
     <row r="184">
@@ -2161,7 +2170,7 @@
         <v>3</v>
       </c>
       <c r="C184" s="0">
-        <v>108.96334838867187</v>
+        <v>108.96334469441564</v>
       </c>
     </row>
     <row r="185">
@@ -2172,7 +2181,7 @@
         <v>4</v>
       </c>
       <c r="C185" s="0">
-        <v>101.40814971923828</v>
+        <v>101.40814734641286</v>
       </c>
     </row>
     <row r="186">
@@ -2183,7 +2192,7 @@
         <v>5</v>
       </c>
       <c r="C186" s="0">
-        <v>72.982437133789063</v>
+        <v>72.982437440336582</v>
       </c>
     </row>
     <row r="187">
@@ -2194,7 +2203,7 @@
         <v>6</v>
       </c>
       <c r="C187" s="0">
-        <v>90.508140563964844</v>
+        <v>90.508135573528975</v>
       </c>
     </row>
     <row r="188">
@@ -2205,7 +2214,7 @@
         <v>7</v>
       </c>
       <c r="C188" s="0">
-        <v>68.187995910644531</v>
+        <v>68.187994849365296</v>
       </c>
     </row>
     <row r="189">
@@ -2216,7 +2225,7 @@
         <v>8</v>
       </c>
       <c r="C189" s="0">
-        <v>91.647727966308594</v>
+        <v>91.647729301347653</v>
       </c>
     </row>
     <row r="190">
@@ -2227,7 +2236,7 @@
         <v>9</v>
       </c>
       <c r="C190" s="0">
-        <v>94.262176513671875</v>
+        <v>94.262173923082898</v>
       </c>
     </row>
     <row r="191">
@@ -2238,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="C191" s="0">
-        <v>110.99637603759766</v>
+        <v>110.99637349305908</v>
       </c>
     </row>
     <row r="192">
@@ -2249,7 +2258,7 @@
         <v>11</v>
       </c>
       <c r="C192" s="0">
-        <v>82.074790954589844</v>
+        <v>82.074792420418262</v>
       </c>
     </row>
     <row r="193">
@@ -2260,7 +2269,7 @@
         <v>12</v>
       </c>
       <c r="C193" s="0">
-        <v>89.423934936523438</v>
+        <v>89.423936228742434</v>
       </c>
     </row>
     <row r="194">
@@ -2271,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="C194" s="0">
-        <v>103.99873352050781</v>
+        <v>103.99873345811896</v>
       </c>
     </row>
     <row r="195">
@@ -2282,7 +2291,7 @@
         <v>2</v>
       </c>
       <c r="C195" s="0">
-        <v>117.69552612304688</v>
+        <v>117.69553222863824</v>
       </c>
     </row>
     <row r="196">
@@ -2293,7 +2302,7 @@
         <v>3</v>
       </c>
       <c r="C196" s="0">
-        <v>111.04788970947266</v>
+        <v>111.0478958953252</v>
       </c>
     </row>
     <row r="197">
@@ -2304,7 +2313,7 @@
         <v>4</v>
       </c>
       <c r="C197" s="0">
-        <v>71.126228332519531</v>
+        <v>71.1262323283146</v>
       </c>
     </row>
     <row r="198">
@@ -2315,7 +2324,7 @@
         <v>5</v>
       </c>
       <c r="C198" s="0">
-        <v>90.164924621582031</v>
+        <v>90.164919466224845</v>
       </c>
     </row>
     <row r="199">
@@ -2326,7 +2335,7 @@
         <v>6</v>
       </c>
       <c r="C199" s="0">
-        <v>68.777374267578125</v>
+        <v>68.777371135066772</v>
       </c>
     </row>
     <row r="200">
@@ -2337,7 +2346,7 @@
         <v>7</v>
       </c>
       <c r="C200" s="0">
-        <v>62.335445404052734</v>
+        <v>62.335446437524098</v>
       </c>
     </row>
     <row r="201">
@@ -2348,7 +2357,7 @@
         <v>8</v>
       </c>
       <c r="C201" s="0">
-        <v>132.47334289550781</v>
+        <v>132.4733321477305</v>
       </c>
     </row>
     <row r="202">
@@ -2359,7 +2368,7 @@
         <v>9</v>
       </c>
       <c r="C202" s="0">
-        <v>176.28372192382812</v>
+        <v>176.28371206161788</v>
       </c>
     </row>
     <row r="203">
@@ -2370,7 +2379,7 @@
         <v>10</v>
       </c>
       <c r="C203" s="0">
-        <v>95.969215393066406</v>
+        <v>95.969213403346714</v>
       </c>
     </row>
     <row r="204">
@@ -2381,7 +2390,7 @@
         <v>11</v>
       </c>
       <c r="C204" s="0">
-        <v>86.566505432128906</v>
+        <v>86.566503465758885</v>
       </c>
     </row>
     <row r="205">
@@ -2392,7 +2401,7 @@
         <v>12</v>
       </c>
       <c r="C205" s="0">
-        <v>121.59109497070312</v>
+        <v>121.59108669531599</v>
       </c>
     </row>
     <row r="206">
@@ -2403,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="C206" s="0">
-        <v>135.73043823242187</v>
+        <v>135.73043577158847</v>
       </c>
     </row>
     <row r="207">
@@ -2414,7 +2423,7 @@
         <v>2</v>
       </c>
       <c r="C207" s="0">
-        <v>119.0836181640625</v>
+        <v>119.08361999195742</v>
       </c>
     </row>
     <row r="208">
@@ -2425,7 +2434,7 @@
         <v>3</v>
       </c>
       <c r="C208" s="0">
-        <v>131.49864196777344</v>
+        <v>131.49864754410734</v>
       </c>
     </row>
     <row r="209">
@@ -2436,7 +2445,7 @@
         <v>4</v>
       </c>
       <c r="C209" s="0">
-        <v>170.47334289550781</v>
+        <v>170.47333251119781</v>
       </c>
     </row>
     <row r="210">
@@ -2447,7 +2456,7 @@
         <v>5</v>
       </c>
       <c r="C210" s="0">
-        <v>140.91246032714844</v>
+        <v>140.91246000958591</v>
       </c>
     </row>
     <row r="211">
@@ -2458,7 +2467,7 @@
         <v>6</v>
       </c>
       <c r="C211" s="0">
-        <v>148.81655883789063</v>
+        <v>148.8165613417035</v>
       </c>
     </row>
     <row r="212">
@@ -2469,7 +2478,7 @@
         <v>7</v>
       </c>
       <c r="C212" s="0">
-        <v>136.10011291503906</v>
+        <v>136.10010571637537</v>
       </c>
     </row>
     <row r="213">
@@ -2480,7 +2489,7 @@
         <v>8</v>
       </c>
       <c r="C213" s="0">
-        <v>86.1436767578125</v>
+        <v>86.143682706913722</v>
       </c>
     </row>
     <row r="214">
@@ -2491,7 +2500,7 @@
         <v>9</v>
       </c>
       <c r="C214" s="0">
-        <v>135.07499694824219</v>
+        <v>135.07500553450706</v>
       </c>
     </row>
     <row r="215">
@@ -2502,7 +2511,7 @@
         <v>10</v>
       </c>
       <c r="C215" s="0">
-        <v>89.914527893066406</v>
+        <v>89.914531399970812</v>
       </c>
     </row>
     <row r="216">
@@ -2513,7 +2522,7 @@
         <v>11</v>
       </c>
       <c r="C216" s="0">
-        <v>120.86214447021484</v>
+        <v>120.86214520248797</v>
       </c>
     </row>
     <row r="217">
@@ -2524,7 +2533,7 @@
         <v>12</v>
       </c>
       <c r="C217" s="0">
-        <v>82.872787475585937</v>
+        <v>82.872786626003631</v>
       </c>
     </row>
     <row r="218">
@@ -2535,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="C218" s="0">
-        <v>135.63230895996094</v>
+        <v>135.63231704946662</v>
       </c>
     </row>
     <row r="219">
@@ -2546,7 +2555,7 @@
         <v>2</v>
       </c>
       <c r="C219" s="0">
-        <v>190.81669616699219</v>
+        <v>190.81671473576529</v>
       </c>
     </row>
     <row r="220">
@@ -2557,7 +2566,7 @@
         <v>3</v>
       </c>
       <c r="C220" s="0">
-        <v>290.92950439453125</v>
+        <v>290.92952088547389</v>
       </c>
     </row>
     <row r="221">
@@ -2568,7 +2577,7 @@
         <v>4</v>
       </c>
       <c r="C221" s="0">
-        <v>197.17079162597656</v>
+        <v>197.17079811515333</v>
       </c>
     </row>
     <row r="222">
@@ -2579,7 +2588,7 @@
         <v>5</v>
       </c>
       <c r="C222" s="0">
-        <v>246.75491333007812</v>
+        <v>246.75490878190044</v>
       </c>
     </row>
     <row r="223">
@@ -2590,7 +2599,7 @@
         <v>6</v>
       </c>
       <c r="C223" s="0">
-        <v>503.94247436523437</v>
+        <v>503.94249242172845</v>
       </c>
     </row>
     <row r="224">
@@ -2601,7 +2610,7 @@
         <v>7</v>
       </c>
       <c r="C224" s="0">
-        <v>558.2236328125</v>
+        <v>558.22364201882272</v>
       </c>
     </row>
     <row r="225">
@@ -2612,7 +2621,7 @@
         <v>8</v>
       </c>
       <c r="C225" s="0">
-        <v>311.36483764648437</v>
+        <v>311.36483202454485</v>
       </c>
     </row>
     <row r="226">
@@ -2623,7 +2632,7 @@
         <v>9</v>
       </c>
       <c r="C226" s="0">
-        <v>209.637939453125</v>
+        <v>209.63793843523842</v>
       </c>
     </row>
     <row r="227">
@@ -2634,7 +2643,7 @@
         <v>10</v>
       </c>
       <c r="C227" s="0">
-        <v>270.02349853515625</v>
+        <v>270.02349186959714</v>
       </c>
     </row>
     <row r="228">
@@ -2645,7 +2654,7 @@
         <v>11</v>
       </c>
       <c r="C228" s="0">
-        <v>358.82839965820312</v>
+        <v>358.82840880746664</v>
       </c>
     </row>
     <row r="229">
@@ -2656,7 +2665,7 @@
         <v>12</v>
       </c>
       <c r="C229" s="0">
-        <v>196.34368896484375</v>
+        <v>196.34369416706684</v>
       </c>
     </row>
     <row r="230">
@@ -2667,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="C230" s="0">
-        <v>257.848388671875</v>
+        <v>257.84839749321475</v>
       </c>
     </row>
     <row r="231">
@@ -2678,7 +2687,7 @@
         <v>2</v>
       </c>
       <c r="C231" s="0">
-        <v>194.04470825195312</v>
+        <v>194.04470490308728</v>
       </c>
     </row>
     <row r="232">
@@ -2689,7 +2698,7 @@
         <v>3</v>
       </c>
       <c r="C232" s="0">
-        <v>232.45973205566406</v>
+        <v>232.45972604144899</v>
       </c>
     </row>
     <row r="233">
@@ -2700,7 +2709,7 @@
         <v>4</v>
       </c>
       <c r="C233" s="0">
-        <v>169.176025390625</v>
+        <v>169.17603591482319</v>
       </c>
     </row>
     <row r="234">
@@ -2711,7 +2720,7 @@
         <v>5</v>
       </c>
       <c r="C234" s="0">
-        <v>159.40144348144531</v>
+        <v>159.40144524851632</v>
       </c>
     </row>
     <row r="235">
@@ -2722,7 +2731,7 @@
         <v>6</v>
       </c>
       <c r="C235" s="0">
-        <v>318.99114990234375</v>
+        <v>318.99116026199204</v>
       </c>
     </row>
     <row r="236">
@@ -2733,7 +2742,7 @@
         <v>7</v>
       </c>
       <c r="C236" s="0">
-        <v>183.65895080566406</v>
+        <v>183.65895058106582</v>
       </c>
     </row>
     <row r="237">
@@ -2744,7 +2753,7 @@
         <v>8</v>
       </c>
       <c r="C237" s="0">
-        <v>151.20429992675781</v>
+        <v>151.20429781015469</v>
       </c>
     </row>
     <row r="238">
@@ -2755,7 +2764,7 @@
         <v>9</v>
       </c>
       <c r="C238" s="0">
-        <v>140.77882385253906</v>
+        <v>140.77881633904866</v>
       </c>
     </row>
     <row r="239">
@@ -2766,7 +2775,7 @@
         <v>10</v>
       </c>
       <c r="C239" s="0">
-        <v>184.03004455566406</v>
+        <v>184.03005097183708</v>
       </c>
     </row>
     <row r="240">
@@ -2777,7 +2786,7 @@
         <v>11</v>
       </c>
       <c r="C240" s="0">
-        <v>214.97006225585938</v>
+        <v>214.97008095639316</v>
       </c>
     </row>
     <row r="241">
@@ -2788,7 +2797,7 @@
         <v>12</v>
       </c>
       <c r="C241" s="0">
-        <v>160.72230529785156</v>
+        <v>160.7223038718837</v>
       </c>
     </row>
     <row r="242">
@@ -2799,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="C242" s="0">
-        <v>123.15999603271484</v>
+        <v>123.1599969116685</v>
       </c>
     </row>
     <row r="243">
@@ -2810,7 +2819,7 @@
         <v>2</v>
       </c>
       <c r="C243" s="0">
-        <v>109.74873352050781</v>
+        <v>109.7487332483494</v>
       </c>
     </row>
     <row r="244">
@@ -2821,7 +2830,7 @@
         <v>3</v>
       </c>
       <c r="C244" s="0">
-        <v>116.60540008544922</v>
+        <v>116.60540265498089</v>
       </c>
     </row>
     <row r="245">
@@ -2832,7 +2841,7 @@
         <v>4</v>
       </c>
       <c r="C245" s="0">
-        <v>102.28702545166016</v>
+        <v>102.28703012879106</v>
       </c>
     </row>
     <row r="246">
@@ -2843,7 +2852,7 @@
         <v>5</v>
       </c>
       <c r="C246" s="0">
-        <v>121.543701171875</v>
+        <v>121.5436956067737</v>
       </c>
     </row>
     <row r="247">
@@ -2854,7 +2863,7 @@
         <v>6</v>
       </c>
       <c r="C247" s="0">
-        <v>105.48676300048828</v>
+        <v>105.48676842316939</v>
       </c>
     </row>
     <row r="248">
@@ -2865,7 +2874,7 @@
         <v>7</v>
       </c>
       <c r="C248" s="0">
-        <v>129.62263488769531</v>
+        <v>129.6226424998398</v>
       </c>
     </row>
     <row r="249">
@@ -2876,7 +2885,7 @@
         <v>8</v>
       </c>
       <c r="C249" s="0">
-        <v>121.62975311279297</v>
+        <v>121.62974835667606</v>
       </c>
     </row>
     <row r="250">
@@ -2887,7 +2896,7 @@
         <v>9</v>
       </c>
       <c r="C250" s="0">
-        <v>157.31582641601562</v>
+        <v>157.31582080050615</v>
       </c>
     </row>
     <row r="251">
@@ -2898,7 +2907,7 @@
         <v>10</v>
       </c>
       <c r="C251" s="0">
-        <v>183.25265502929687</v>
+        <v>183.25266625551419</v>
       </c>
     </row>
     <row r="252">
@@ -2909,7 +2918,7 @@
         <v>11</v>
       </c>
       <c r="C252" s="0">
-        <v>191.96647644042969</v>
+        <v>191.96645652769618</v>
       </c>
     </row>
     <row r="253">
@@ -2920,7 +2929,7 @@
         <v>12</v>
       </c>
       <c r="C253" s="0">
-        <v>239.69102478027344</v>
+        <v>239.69102981938227</v>
       </c>
     </row>
     <row r="254">
@@ -2931,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="C254" s="0">
-        <v>309.97244262695312</v>
+        <v>309.97244945797701</v>
       </c>
     </row>
     <row r="255">
@@ -2942,7 +2951,7 @@
         <v>2</v>
       </c>
       <c r="C255" s="0">
-        <v>196.95947265625</v>
+        <v>196.95946459830401</v>
       </c>
     </row>
     <row r="256">
@@ -2953,7 +2962,7 @@
         <v>3</v>
       </c>
       <c r="C256" s="0">
-        <v>212.78254699707031</v>
+        <v>212.78254189044787</v>
       </c>
     </row>
     <row r="257">
@@ -2964,7 +2973,7 @@
         <v>4</v>
       </c>
       <c r="C257" s="0">
-        <v>135.51847839355469</v>
+        <v>135.51848003853243</v>
       </c>
     </row>
     <row r="258">
@@ -2975,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="C258" s="0">
-        <v>158.68260192871094</v>
+        <v>158.68260551719968</v>
       </c>
     </row>
     <row r="259">
@@ -2986,7 +2995,7 @@
         <v>6</v>
       </c>
       <c r="C259" s="0">
-        <v>149.80560302734375</v>
+        <v>149.80560130108137</v>
       </c>
     </row>
     <row r="260">
@@ -2997,7 +3006,7 @@
         <v>7</v>
       </c>
       <c r="C260" s="0">
-        <v>202.04379272460938</v>
+        <v>202.04377955585122</v>
       </c>
     </row>
     <row r="261">
@@ -3008,7 +3017,7 @@
         <v>8</v>
       </c>
       <c r="C261" s="0">
-        <v>238.91572570800781</v>
+        <v>238.91571234839765</v>
       </c>
     </row>
     <row r="262">
@@ -3019,7 +3028,7 @@
         <v>9</v>
       </c>
       <c r="C262" s="0">
-        <v>187.41012573242187</v>
+        <v>187.41011632363401</v>
       </c>
     </row>
     <row r="263">
@@ -3030,7 +3039,7 @@
         <v>10</v>
       </c>
       <c r="C263" s="0">
-        <v>233.31156921386719</v>
+        <v>233.31156413860188</v>
       </c>
     </row>
     <row r="264">
@@ -3041,7 +3050,7 @@
         <v>11</v>
       </c>
       <c r="C264" s="0">
-        <v>205.59706115722656</v>
+        <v>205.59707355365967</v>
       </c>
     </row>
     <row r="265">
@@ -3052,7 +3061,7 @@
         <v>12</v>
       </c>
       <c r="C265" s="0">
-        <v>271.30404663085937</v>
+        <v>271.30406158523687</v>
       </c>
     </row>
     <row r="266">
@@ -3063,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="C266" s="0">
-        <v>198.156494140625</v>
+        <v>198.15649141819117</v>
       </c>
     </row>
     <row r="267">
@@ -3074,7 +3083,7 @@
         <v>2</v>
       </c>
       <c r="C267" s="0">
-        <v>139.62191772460937</v>
+        <v>139.62192204074458</v>
       </c>
     </row>
     <row r="268">
@@ -3085,7 +3094,7 @@
         <v>3</v>
       </c>
       <c r="C268" s="0">
-        <v>281.207275390625</v>
+        <v>281.20727140397986</v>
       </c>
     </row>
     <row r="269">
@@ -3096,7 +3105,7 @@
         <v>4</v>
       </c>
       <c r="C269" s="0">
-        <v>185.35208129882812</v>
+        <v>185.35208283420195</v>
       </c>
     </row>
     <row r="270">
@@ -3107,7 +3116,7 @@
         <v>5</v>
       </c>
       <c r="C270" s="0">
-        <v>230.75636291503906</v>
+        <v>230.75636037309954</v>
       </c>
     </row>
     <row r="271">
@@ -3118,7 +3127,7 @@
         <v>6</v>
       </c>
       <c r="C271" s="0">
-        <v>167.69786071777344</v>
+        <v>167.69786380940585</v>
       </c>
     </row>
     <row r="272">
@@ -3129,7 +3138,7 @@
         <v>7</v>
       </c>
       <c r="C272" s="0">
-        <v>189.96194458007812</v>
+        <v>189.96193934251556</v>
       </c>
     </row>
     <row r="273">
@@ -3140,7 +3149,7 @@
         <v>8</v>
       </c>
       <c r="C273" s="0">
-        <v>176.54884338378906</v>
+        <v>176.54884283733892</v>
       </c>
     </row>
     <row r="274">
@@ -3151,7 +3160,7 @@
         <v>9</v>
       </c>
       <c r="C274" s="0">
-        <v>184.51463317871094</v>
+        <v>184.51675172929453</v>
       </c>
     </row>
     <row r="275">
@@ -3162,15 +3171,334 @@
         <v>10</v>
       </c>
       <c r="C275" s="0">
-        <v>181.37814331054687</v>
+        <v>189.1247735854013</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
+        <v>23</v>
+      </c>
+      <c r="B276" s="0">
+        <v>11</v>
+      </c>
+      <c r="C276" s="0">
+        <v>214.46165401121681</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>23</v>
+      </c>
+      <c r="B277" s="0">
+        <v>12</v>
+      </c>
+      <c r="C277" s="0">
+        <v>207.60650804572748</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
         <v>24</v>
       </c>
-      <c r="B276" s="0"/>
-      <c r="C276" s="0"/>
+      <c r="B278" s="0">
+        <v>1</v>
+      </c>
+      <c r="C278" s="0">
+        <v>112.63905727443453</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>24</v>
+      </c>
+      <c r="B279" s="0">
+        <v>2</v>
+      </c>
+      <c r="C279" s="0">
+        <v>138.00994636357206</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>24</v>
+      </c>
+      <c r="B280" s="0">
+        <v>3</v>
+      </c>
+      <c r="C280" s="0">
+        <v>142.40594412833096</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>24</v>
+      </c>
+      <c r="B281" s="0">
+        <v>4</v>
+      </c>
+      <c r="C281" s="0">
+        <v>95.280677239972462</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>24</v>
+      </c>
+      <c r="B282" s="0">
+        <v>5</v>
+      </c>
+      <c r="C282" s="0">
+        <v>98.11193470584746</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>24</v>
+      </c>
+      <c r="B283" s="0">
+        <v>6</v>
+      </c>
+      <c r="C283" s="0">
+        <v>90.334937611228654</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>24</v>
+      </c>
+      <c r="B284" s="0">
+        <v>7</v>
+      </c>
+      <c r="C284" s="0">
+        <v>88.283767152168153</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>24</v>
+      </c>
+      <c r="B285" s="0">
+        <v>8</v>
+      </c>
+      <c r="C285" s="0">
+        <v>79.109103716265921</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>24</v>
+      </c>
+      <c r="B286" s="0">
+        <v>9</v>
+      </c>
+      <c r="C286" s="0">
+        <v>78.700928887261341</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>24</v>
+      </c>
+      <c r="B287" s="0">
+        <v>10</v>
+      </c>
+      <c r="C287" s="0">
+        <v>103.9897920730636</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>24</v>
+      </c>
+      <c r="B288" s="0">
+        <v>11</v>
+      </c>
+      <c r="C288" s="0">
+        <v>75.317495277532174</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>24</v>
+      </c>
+      <c r="B289" s="0">
+        <v>12</v>
+      </c>
+      <c r="C289" s="0">
+        <v>174.83133982207281</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>25</v>
+      </c>
+      <c r="B290" s="0">
+        <v>1</v>
+      </c>
+      <c r="C290" s="0">
+        <v>88.199173561725758</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>25</v>
+      </c>
+      <c r="B291" s="0">
+        <v>2</v>
+      </c>
+      <c r="C291" s="0">
+        <v>80.71515390083168</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>25</v>
+      </c>
+      <c r="B292" s="0">
+        <v>3</v>
+      </c>
+      <c r="C292" s="0">
+        <v>170.0450385906353</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>25</v>
+      </c>
+      <c r="B293" s="0">
+        <v>4</v>
+      </c>
+      <c r="C293" s="0">
+        <v>123.43514711846839</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>25</v>
+      </c>
+      <c r="B294" s="0">
+        <v>5</v>
+      </c>
+      <c r="C294" s="0">
+        <v>105.19512401227369</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>25</v>
+      </c>
+      <c r="B295" s="0">
+        <v>6</v>
+      </c>
+      <c r="C295" s="0">
+        <v>118.81205960472241</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>25</v>
+      </c>
+      <c r="B296" s="0">
+        <v>7</v>
+      </c>
+      <c r="C296" s="0">
+        <v>184.27249051796957</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>25</v>
+      </c>
+      <c r="B297" s="0">
+        <v>8</v>
+      </c>
+      <c r="C297" s="0">
+        <v>124.28907856525075</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>25</v>
+      </c>
+      <c r="B298" s="0">
+        <v>9</v>
+      </c>
+      <c r="C298" s="0">
+        <v>230.05940534595089</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>25</v>
+      </c>
+      <c r="B299" s="0">
+        <v>10</v>
+      </c>
+      <c r="C299" s="0">
+        <v>399.80611032798606</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>25</v>
+      </c>
+      <c r="B300" s="0">
+        <v>11</v>
+      </c>
+      <c r="C300" s="0">
+        <v>220.10555967592006</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>25</v>
+      </c>
+      <c r="B301" s="0">
+        <v>12</v>
+      </c>
+      <c r="C301" s="0">
+        <v>167.63100925224853</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>26</v>
+      </c>
+      <c r="B302" s="0">
+        <v>1</v>
+      </c>
+      <c r="C302" s="0">
+        <v>140.0670895461748</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>26</v>
+      </c>
+      <c r="B303" s="0">
+        <v>2</v>
+      </c>
+      <c r="C303" s="0">
+        <v>121.21055490453543</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>26</v>
+      </c>
+      <c r="B304" s="0">
+        <v>3</v>
+      </c>
+      <c r="C304" s="0">
+        <v>133.19809057072493</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>27</v>
+      </c>
+      <c r="B305" s="0"/>
+      <c r="C305" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>